<commit_message>
ftp upload fix for java code.
</commit_message>
<xml_diff>
--- a/test_scripts/chrome/QS006_demoqa_testscript.xlsx
+++ b/test_scripts/chrome/QS006_demoqa_testscript.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\java-projects\webautomationframework_java\test_scripts\chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D2510B-62D5-4704-8D9C-E9AD64B21F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517B8EBB-6A23-4CDC-BC07-418644A1EE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>open_browser</t>
   </si>
@@ -272,9 +272,6 @@
   </si>
   <si>
     <t>demoqa_home_form_sub_close_css</t>
-  </si>
-  <si>
-    <t>chromedgerunonlinux.txt</t>
   </si>
 </sst>
 </file>
@@ -657,7 +654,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,9 +1003,6 @@
       <c r="C30" t="s">
         <v>64</v>
       </c>
-      <c r="D30" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="31" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">

</xml_diff>